<commit_message>
more setup of models
</commit_message>
<xml_diff>
--- a/db/sources/system_permissions.xlsx
+++ b/db/sources/system_permissions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wrburgess/Projects/aaa/kc-tennis/db/source/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wrburgess/Projects/mpi/harvest/db/sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E8FE88-52A4-F445-973A-A5630CBE3EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60F2C5F-FFAA-8F4B-8675-D17775304C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="660" windowWidth="37160" windowHeight="20780" xr2:uid="{A7924D65-00DE-2544-9F97-E11FDD26EDD2}"/>
+    <workbookView xWindow="1080" yWindow="660" windowWidth="37160" windowHeight="20780" activeTab="3" xr2:uid="{A7924D65-00DE-2544-9F97-E11FDD26EDD2}"/>
   </bookViews>
   <sheets>
     <sheet name="system_permissions" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="56">
   <si>
     <t>Contact</t>
   </si>
@@ -191,13 +191,19 @@
     <t>member_export_xlsx</t>
   </si>
   <si>
-    <t>wrburgess@gmail.com</t>
-  </si>
-  <si>
     <t>copy</t>
   </si>
   <si>
     <t>archive</t>
+  </si>
+  <si>
+    <t>rburgess@mpimedia.com</t>
+  </si>
+  <si>
+    <t>dennis@dennmart.com</t>
+  </si>
+  <si>
+    <t>badie@mpimedia.com</t>
   </si>
 </sst>
 </file>
@@ -1095,7 +1101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6930FAF-2397-5948-B560-84F685BD8951}">
   <dimension ref="A1:C125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+    <sheetView topLeftCell="A89" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -1221,7 +1227,7 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>15</v>
@@ -1430,7 +1436,7 @@
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>15</v>
@@ -1661,7 +1667,7 @@
         <v>5</v>
       </c>
       <c r="B51" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>15</v>
@@ -2079,7 +2085,7 @@
         <v>8</v>
       </c>
       <c r="B89" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>15</v>
@@ -2299,7 +2305,7 @@
         <v>10</v>
       </c>
       <c r="B109" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>15</v>
@@ -2464,7 +2470,7 @@
         <v>4</v>
       </c>
       <c r="B124" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>15</v>
@@ -2660,8 +2666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2563C8-FCA3-B346-8303-FDE8EF30B49B}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2680,9 +2686,25 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2701,6 +2723,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{CC29CB2C-A123-884B-AA67-2BA30331EC14}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{52105717-854C-6142-8740-CCBD87185901}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{EAC4EE52-CEB6-AF4E-90FB-51A28FDB7B20}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>